<commit_message>
setting for host and delete version for requirements.txt
</commit_message>
<xml_diff>
--- a/data/unknown-questions.xlsx
+++ b/data/unknown-questions.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -520,7 +520,7 @@
         </is>
       </c>
       <c r="B8" s="2" t="n">
-        <v>46043.44030384883</v>
+        <v>46043.44030385416</v>
       </c>
     </row>
     <row r="9">
@@ -530,7 +530,17 @@
         </is>
       </c>
       <c r="B9" s="2" t="n">
-        <v>46043.440869819</v>
+        <v>46043.44086981482</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>lupa password master</t>
+        </is>
+      </c>
+      <c r="B10" s="2" t="n">
+        <v>46045.62859663679</v>
       </c>
     </row>
   </sheetData>

</xml_diff>